<commit_message>
Added for Diagnostic Report
</commit_message>
<xml_diff>
--- a/FHIR-Profiling.xlsx
+++ b/FHIR-Profiling.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t xml:space="preserve">Actors </t>
   </si>
@@ -115,9 +115,6 @@
     <t>FHIR Resource</t>
   </si>
   <si>
-    <t>DiagnosticReport/Composition</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -209,6 +206,12 @@
   </si>
   <si>
     <t>Can be specified by bodysite coe</t>
+  </si>
+  <si>
+    <t>When observation, expected value is binary - Yes/No, True/False</t>
+  </si>
+  <si>
+    <t>DiagnosticReport/Composition/Specimen</t>
   </si>
 </sst>
 </file>
@@ -271,9 +274,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -281,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -607,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,7 +619,7 @@
     <col min="1" max="1" width="27.26953125" customWidth="1"/>
     <col min="2" max="2" width="23.1796875" customWidth="1"/>
     <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="36.90625" customWidth="1"/>
     <col min="5" max="5" width="36.6328125" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.36328125" customWidth="1"/>
     <col min="7" max="7" width="11.26953125" customWidth="1"/>
@@ -628,20 +631,20 @@
         <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -651,52 +654,58 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+      <c r="A3" s="7"/>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
+      <c r="A4" s="7"/>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="A5" s="7"/>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="A6" s="7"/>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="A7" s="7"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -715,191 +724,194 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>60</v>
+        <v>31</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="G11" s="3">
         <v>49727002</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>56</v>
+      <c r="H11" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="7"/>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
         <v>49</v>
-      </c>
-      <c r="F12" t="s">
-        <v>50</v>
       </c>
       <c r="G12">
         <v>62315008</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="7"/>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13">
         <v>249497008</v>
       </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="7"/>
       <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15">
         <v>267036007</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
+      <c r="A16" s="7"/>
       <c r="B16" t="s">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>58</v>
+        <v>31</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
+      <c r="A17" s="7"/>
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+      <c r="A18" s="7"/>
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
+      <c r="A19" s="7"/>
       <c r="B19" t="s">
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
+      <c r="A20" s="7"/>
       <c r="B20" t="s">
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+      <c r="A21" s="7"/>
       <c r="B21" t="s">
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
+      <c r="A22" s="7"/>
       <c r="B22" t="s">
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
+      <c r="A23" s="7"/>
       <c r="B23" t="s">
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -907,77 +919,77 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1472,16 +1484,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E8D402-6D3A-40F9-9F5C-5AF00CAF8334}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="61c5f8ff-6d52-4b37-b0e6-6f7f31ff08ca"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b494b8ef-4353-4d1b-b9cb-2876ad3d974a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b494b8ef-4353-4d1b-b9cb-2876ad3d974a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="61c5f8ff-6d52-4b37-b0e6-6f7f31ff08ca"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>